<commit_message>
Added request for valves specification availability
</commit_message>
<xml_diff>
--- a/input/Templates/Template-MPD0001.xlsx
+++ b/input/Templates/Template-MPD0001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\PycharmProjects\pythonProject2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\PycharmProjects\pipelines-insulation\input\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">ПОЗ.
 </t>
@@ -133,6 +133,9 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Ведомость теплоизоляционных конструкций</t>
+  </si>
 </sst>
 </file>
 
@@ -152,12 +155,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="20"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -202,6 +199,13 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -277,23 +281,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -314,34 +318,34 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -352,42 +356,41 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -707,7 +710,7 @@
   <dimension ref="A1:W842"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -727,67 +730,69 @@
     <col min="13" max="13" width="34" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
+    <row r="1" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:23" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="45" t="s">
+      <c r="J2" s="50"/>
+      <c r="K2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="42" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="48" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="43"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
@@ -800,9 +805,9 @@
       <c r="L3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="43"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="50"/>
+      <c r="M3" s="44"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="42"/>
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12676,8 +12681,8 @@
       <c r="H792" s="26"/>
       <c r="I792" s="35"/>
       <c r="J792" s="36"/>
-      <c r="K792" s="53"/>
-      <c r="L792" s="53"/>
+      <c r="K792" s="40"/>
+      <c r="L792" s="40"/>
       <c r="M792" s="37"/>
     </row>
     <row r="793" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12691,8 +12696,8 @@
       <c r="H793" s="26"/>
       <c r="I793" s="35"/>
       <c r="J793" s="36"/>
-      <c r="K793" s="53"/>
-      <c r="L793" s="53"/>
+      <c r="K793" s="40"/>
+      <c r="L793" s="40"/>
       <c r="M793" s="37"/>
     </row>
     <row r="794" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12706,8 +12711,8 @@
       <c r="H794" s="26"/>
       <c r="I794" s="35"/>
       <c r="J794" s="36"/>
-      <c r="K794" s="53"/>
-      <c r="L794" s="53"/>
+      <c r="K794" s="40"/>
+      <c r="L794" s="40"/>
       <c r="M794" s="37"/>
     </row>
     <row r="795" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12721,8 +12726,8 @@
       <c r="H795" s="26"/>
       <c r="I795" s="35"/>
       <c r="J795" s="36"/>
-      <c r="K795" s="53"/>
-      <c r="L795" s="53"/>
+      <c r="K795" s="40"/>
+      <c r="L795" s="40"/>
       <c r="M795" s="37"/>
     </row>
     <row r="796" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12736,8 +12741,8 @@
       <c r="H796" s="26"/>
       <c r="I796" s="35"/>
       <c r="J796" s="36"/>
-      <c r="K796" s="53"/>
-      <c r="L796" s="53"/>
+      <c r="K796" s="40"/>
+      <c r="L796" s="40"/>
       <c r="M796" s="37"/>
     </row>
     <row r="797" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12751,8 +12756,8 @@
       <c r="H797" s="26"/>
       <c r="I797" s="35"/>
       <c r="J797" s="36"/>
-      <c r="K797" s="53"/>
-      <c r="L797" s="53"/>
+      <c r="K797" s="40"/>
+      <c r="L797" s="40"/>
       <c r="M797" s="37"/>
     </row>
     <row r="798" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12766,8 +12771,8 @@
       <c r="H798" s="26"/>
       <c r="I798" s="35"/>
       <c r="J798" s="36"/>
-      <c r="K798" s="53"/>
-      <c r="L798" s="53"/>
+      <c r="K798" s="40"/>
+      <c r="L798" s="40"/>
       <c r="M798" s="37"/>
     </row>
     <row r="799" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12781,8 +12786,8 @@
       <c r="H799" s="26"/>
       <c r="I799" s="35"/>
       <c r="J799" s="36"/>
-      <c r="K799" s="53"/>
-      <c r="L799" s="53"/>
+      <c r="K799" s="40"/>
+      <c r="L799" s="40"/>
       <c r="M799" s="37"/>
     </row>
     <row r="800" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12796,8 +12801,8 @@
       <c r="H800" s="26"/>
       <c r="I800" s="35"/>
       <c r="J800" s="36"/>
-      <c r="K800" s="53"/>
-      <c r="L800" s="53"/>
+      <c r="K800" s="40"/>
+      <c r="L800" s="40"/>
       <c r="M800" s="37"/>
     </row>
     <row r="801" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12811,8 +12816,8 @@
       <c r="H801" s="26"/>
       <c r="I801" s="35"/>
       <c r="J801" s="36"/>
-      <c r="K801" s="53"/>
-      <c r="L801" s="53"/>
+      <c r="K801" s="40"/>
+      <c r="L801" s="40"/>
       <c r="M801" s="37"/>
     </row>
     <row r="802" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12826,8 +12831,8 @@
       <c r="H802" s="26"/>
       <c r="I802" s="35"/>
       <c r="J802" s="36"/>
-      <c r="K802" s="53"/>
-      <c r="L802" s="53"/>
+      <c r="K802" s="40"/>
+      <c r="L802" s="40"/>
       <c r="M802" s="37"/>
     </row>
     <row r="803" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12841,8 +12846,8 @@
       <c r="H803" s="26"/>
       <c r="I803" s="35"/>
       <c r="J803" s="36"/>
-      <c r="K803" s="53"/>
-      <c r="L803" s="53"/>
+      <c r="K803" s="40"/>
+      <c r="L803" s="40"/>
       <c r="M803" s="37"/>
     </row>
     <row r="804" spans="1:13" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -12856,8 +12861,8 @@
       <c r="H804" s="26"/>
       <c r="I804" s="35"/>
       <c r="J804" s="36"/>
-      <c r="K804" s="53"/>
-      <c r="L804" s="53"/>
+      <c r="K804" s="40"/>
+      <c r="L804" s="40"/>
       <c r="M804" s="37"/>
     </row>
     <row r="805" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12871,8 +12876,8 @@
       <c r="H805" s="26"/>
       <c r="I805" s="35"/>
       <c r="J805" s="36"/>
-      <c r="K805" s="53"/>
-      <c r="L805" s="53"/>
+      <c r="K805" s="40"/>
+      <c r="L805" s="40"/>
       <c r="M805" s="37"/>
     </row>
     <row r="806" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12886,8 +12891,8 @@
       <c r="H806" s="26"/>
       <c r="I806" s="35"/>
       <c r="J806" s="36"/>
-      <c r="K806" s="53"/>
-      <c r="L806" s="53"/>
+      <c r="K806" s="40"/>
+      <c r="L806" s="40"/>
       <c r="M806" s="37"/>
     </row>
     <row r="807" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12901,8 +12906,8 @@
       <c r="H807" s="26"/>
       <c r="I807" s="35"/>
       <c r="J807" s="36"/>
-      <c r="K807" s="53"/>
-      <c r="L807" s="53"/>
+      <c r="K807" s="40"/>
+      <c r="L807" s="40"/>
       <c r="M807" s="37"/>
     </row>
     <row r="808" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12916,8 +12921,8 @@
       <c r="H808" s="26"/>
       <c r="I808" s="35"/>
       <c r="J808" s="36"/>
-      <c r="K808" s="53"/>
-      <c r="L808" s="53"/>
+      <c r="K808" s="40"/>
+      <c r="L808" s="40"/>
       <c r="M808" s="37"/>
     </row>
     <row r="809" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12931,8 +12936,8 @@
       <c r="H809" s="26"/>
       <c r="I809" s="35"/>
       <c r="J809" s="36"/>
-      <c r="K809" s="53"/>
-      <c r="L809" s="53"/>
+      <c r="K809" s="40"/>
+      <c r="L809" s="40"/>
       <c r="M809" s="37"/>
     </row>
     <row r="810" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12946,8 +12951,8 @@
       <c r="H810" s="26"/>
       <c r="I810" s="35"/>
       <c r="J810" s="36"/>
-      <c r="K810" s="53"/>
-      <c r="L810" s="53"/>
+      <c r="K810" s="40"/>
+      <c r="L810" s="40"/>
       <c r="M810" s="37"/>
     </row>
     <row r="811" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12961,8 +12966,8 @@
       <c r="H811" s="26"/>
       <c r="I811" s="35"/>
       <c r="J811" s="36"/>
-      <c r="K811" s="53"/>
-      <c r="L811" s="53"/>
+      <c r="K811" s="40"/>
+      <c r="L811" s="40"/>
       <c r="M811" s="37"/>
     </row>
     <row r="812" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12976,8 +12981,8 @@
       <c r="H812" s="26"/>
       <c r="I812" s="35"/>
       <c r="J812" s="36"/>
-      <c r="K812" s="53"/>
-      <c r="L812" s="53"/>
+      <c r="K812" s="40"/>
+      <c r="L812" s="40"/>
       <c r="M812" s="37"/>
     </row>
     <row r="813" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -12991,8 +12996,8 @@
       <c r="H813" s="26"/>
       <c r="I813" s="35"/>
       <c r="J813" s="36"/>
-      <c r="K813" s="53"/>
-      <c r="L813" s="53"/>
+      <c r="K813" s="40"/>
+      <c r="L813" s="40"/>
       <c r="M813" s="37"/>
     </row>
     <row r="814" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -13006,8 +13011,8 @@
       <c r="H814" s="26"/>
       <c r="I814" s="35"/>
       <c r="J814" s="36"/>
-      <c r="K814" s="53"/>
-      <c r="L814" s="53"/>
+      <c r="K814" s="40"/>
+      <c r="L814" s="40"/>
       <c r="M814" s="37"/>
     </row>
     <row r="815" spans="1:13" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -13021,8 +13026,8 @@
       <c r="H815" s="26"/>
       <c r="I815" s="35"/>
       <c r="J815" s="36"/>
-      <c r="K815" s="53"/>
-      <c r="L815" s="53"/>
+      <c r="K815" s="40"/>
+      <c r="L815" s="40"/>
       <c r="M815" s="37"/>
     </row>
     <row r="816" spans="1:13" s="28" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -13036,8 +13041,8 @@
       <c r="H816" s="26"/>
       <c r="I816" s="35"/>
       <c r="J816" s="36"/>
-      <c r="K816" s="53"/>
-      <c r="L816" s="53"/>
+      <c r="K816" s="40"/>
+      <c r="L816" s="40"/>
       <c r="M816" s="37"/>
     </row>
     <row r="817" spans="1:20" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -13051,8 +13056,8 @@
       <c r="H817" s="26"/>
       <c r="I817" s="35"/>
       <c r="J817" s="36"/>
-      <c r="K817" s="53"/>
-      <c r="L817" s="53"/>
+      <c r="K817" s="40"/>
+      <c r="L817" s="40"/>
       <c r="M817" s="37"/>
     </row>
     <row r="818" spans="1:20" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -13066,8 +13071,8 @@
       <c r="H818" s="26"/>
       <c r="I818" s="35"/>
       <c r="J818" s="36"/>
-      <c r="K818" s="53"/>
-      <c r="L818" s="53"/>
+      <c r="K818" s="40"/>
+      <c r="L818" s="40"/>
       <c r="M818" s="37"/>
     </row>
     <row r="819" spans="1:20" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -13081,8 +13086,8 @@
       <c r="H819" s="26"/>
       <c r="I819" s="35"/>
       <c r="J819" s="36"/>
-      <c r="K819" s="53"/>
-      <c r="L819" s="53"/>
+      <c r="K819" s="40"/>
+      <c r="L819" s="40"/>
       <c r="M819" s="37"/>
     </row>
     <row r="820" spans="1:20" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -13096,8 +13101,8 @@
       <c r="H820" s="26"/>
       <c r="I820" s="35"/>
       <c r="J820" s="36"/>
-      <c r="K820" s="53"/>
-      <c r="L820" s="53"/>
+      <c r="K820" s="40"/>
+      <c r="L820" s="40"/>
       <c r="M820" s="37"/>
     </row>
     <row r="821" spans="1:20" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -13111,8 +13116,8 @@
       <c r="H821" s="26"/>
       <c r="I821" s="35"/>
       <c r="J821" s="36"/>
-      <c r="K821" s="53"/>
-      <c r="L821" s="53"/>
+      <c r="K821" s="40"/>
+      <c r="L821" s="40"/>
       <c r="M821" s="37"/>
     </row>
     <row r="822" spans="1:20" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -13126,8 +13131,8 @@
       <c r="H822" s="26"/>
       <c r="I822" s="35"/>
       <c r="J822" s="36"/>
-      <c r="K822" s="53"/>
-      <c r="L822" s="53"/>
+      <c r="K822" s="40"/>
+      <c r="L822" s="40"/>
       <c r="M822" s="37"/>
     </row>
     <row r="823" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13141,8 +13146,8 @@
       <c r="H823" s="26"/>
       <c r="I823" s="35"/>
       <c r="J823" s="36"/>
-      <c r="K823" s="53"/>
-      <c r="L823" s="53"/>
+      <c r="K823" s="40"/>
+      <c r="L823" s="40"/>
       <c r="M823" s="37"/>
     </row>
     <row r="824" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13156,8 +13161,8 @@
       <c r="H824" s="26"/>
       <c r="I824" s="35"/>
       <c r="J824" s="36"/>
-      <c r="K824" s="53"/>
-      <c r="L824" s="53"/>
+      <c r="K824" s="40"/>
+      <c r="L824" s="40"/>
       <c r="M824" s="37"/>
     </row>
     <row r="825" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13171,8 +13176,8 @@
       <c r="H825" s="26"/>
       <c r="I825" s="35"/>
       <c r="J825" s="36"/>
-      <c r="K825" s="53"/>
-      <c r="L825" s="53"/>
+      <c r="K825" s="40"/>
+      <c r="L825" s="40"/>
       <c r="M825" s="37"/>
       <c r="T825" s="29"/>
     </row>
@@ -13187,8 +13192,8 @@
       <c r="H826" s="26"/>
       <c r="I826" s="35"/>
       <c r="J826" s="36"/>
-      <c r="K826" s="53"/>
-      <c r="L826" s="53"/>
+      <c r="K826" s="40"/>
+      <c r="L826" s="40"/>
       <c r="M826" s="37"/>
       <c r="R826" s="38"/>
       <c r="T826" s="30"/>
@@ -13204,8 +13209,8 @@
       <c r="H827" s="26"/>
       <c r="I827" s="35"/>
       <c r="J827" s="36"/>
-      <c r="K827" s="53"/>
-      <c r="L827" s="53"/>
+      <c r="K827" s="40"/>
+      <c r="L827" s="40"/>
       <c r="M827" s="37"/>
     </row>
     <row r="828" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13219,8 +13224,8 @@
       <c r="H828" s="26"/>
       <c r="I828" s="35"/>
       <c r="J828" s="36"/>
-      <c r="K828" s="53"/>
-      <c r="L828" s="53"/>
+      <c r="K828" s="40"/>
+      <c r="L828" s="40"/>
       <c r="M828" s="37"/>
     </row>
     <row r="829" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13234,8 +13239,8 @@
       <c r="H829" s="26"/>
       <c r="I829" s="35"/>
       <c r="J829" s="36"/>
-      <c r="K829" s="53"/>
-      <c r="L829" s="53"/>
+      <c r="K829" s="40"/>
+      <c r="L829" s="40"/>
       <c r="M829" s="37"/>
     </row>
     <row r="830" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13249,8 +13254,8 @@
       <c r="H830" s="26"/>
       <c r="I830" s="35"/>
       <c r="J830" s="36"/>
-      <c r="K830" s="53"/>
-      <c r="L830" s="53"/>
+      <c r="K830" s="40"/>
+      <c r="L830" s="40"/>
       <c r="M830" s="37"/>
     </row>
     <row r="831" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13264,8 +13269,8 @@
       <c r="H831" s="26"/>
       <c r="I831" s="35"/>
       <c r="J831" s="36"/>
-      <c r="K831" s="53"/>
-      <c r="L831" s="53"/>
+      <c r="K831" s="40"/>
+      <c r="L831" s="40"/>
       <c r="M831" s="37"/>
     </row>
     <row r="832" spans="1:20" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13279,8 +13284,8 @@
       <c r="H832" s="26"/>
       <c r="I832" s="35"/>
       <c r="J832" s="36"/>
-      <c r="K832" s="53"/>
-      <c r="L832" s="53"/>
+      <c r="K832" s="40"/>
+      <c r="L832" s="40"/>
       <c r="M832" s="37"/>
     </row>
     <row r="833" spans="1:13" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13294,8 +13299,8 @@
       <c r="H833" s="26"/>
       <c r="I833" s="35"/>
       <c r="J833" s="36"/>
-      <c r="K833" s="53"/>
-      <c r="L833" s="53"/>
+      <c r="K833" s="40"/>
+      <c r="L833" s="40"/>
       <c r="M833" s="37"/>
     </row>
     <row r="834" spans="1:13" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13309,8 +13314,8 @@
       <c r="H834" s="26"/>
       <c r="I834" s="35"/>
       <c r="J834" s="36"/>
-      <c r="K834" s="53"/>
-      <c r="L834" s="53"/>
+      <c r="K834" s="40"/>
+      <c r="L834" s="40"/>
       <c r="M834" s="37"/>
     </row>
     <row r="835" spans="1:13" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -13407,12 +13412,6 @@
     <row r="842" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="F2:F3"/>
@@ -13420,6 +13419,12 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.98425196850393704" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.55118110236220474"/>
   <pageSetup paperSize="8" scale="88" orientation="landscape" r:id="rId1"/>

</xml_diff>